<commit_message>
Update for Wed May 31 15:41:01 2023
</commit_message>
<xml_diff>
--- a/distros/S/Spreadsheet-Edit/tlib/Test.xlsx
+++ b/distros/S/Spreadsheet-Edit/tlib/Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t xml:space="preserve">mary.jones@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Françoise-Athénaïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de Rochechouart</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
@@ -166,8 +172,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -203,18 +209,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,6 +263,17 @@
       </c>
       <c r="D3" s="1" t="n">
         <v>37145</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-94683</v>
       </c>
     </row>
   </sheetData>
@@ -281,8 +298,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="A1:C13 G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,15 +309,15 @@
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="n">
         <v>100</v>
@@ -308,7 +325,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>101</v>
@@ -316,7 +333,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="n">
         <v>102</v>
@@ -324,7 +341,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>103</v>
@@ -332,7 +349,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>104</v>

</xml_diff>

<commit_message>
Update for Tue Oct 15 05:06:53 2024
</commit_message>
<xml_diff>
--- a/distros/S/Spreadsheet-Edit/tlib/Test.xlsx
+++ b/distros/S/Spreadsheet-Edit/tlib/Test.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Another Sheet" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Another Sheet" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
+    <t xml:space="preserve">Zipcode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joe</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
     <t xml:space="preserve">joe@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">00000</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mary</t>
   </si>
   <si>
@@ -53,10 +59,16 @@
     <t xml:space="preserve">mary.jones@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">12345</t>
+  </si>
+  <si>
     <t xml:space="preserve">Françoise-Athénaïs</t>
   </si>
   <si>
     <t xml:space="preserve">de Rochechouart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00007</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
@@ -84,9 +96,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mmm\ d&quot;, &quot;yyyy"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -167,28 +180,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,76 +229,195 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="A1:C13"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="12.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>44562</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>37145</v>
       </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>-94683</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -292,66 +436,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="1" sqref="A1:C13 G5"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="8" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
+    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="n">
+      <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="n">
+      <c r="A3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8" t="n">
         <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="5" t="n">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="5" t="n">
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="8" t="n">
         <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="n">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8" t="n">
         <v>104</v>
       </c>
     </row>

</xml_diff>